<commit_message>
wrote questions for manage
</commit_message>
<xml_diff>
--- a/Semester02_AssessmentPlan .xlsx
+++ b/Semester02_AssessmentPlan .xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre\Desktop\Tafe-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre\Desktop\Tafe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CAF5E2-215B-460C-B800-897CB0440D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D211FD1-6B42-434E-B1CD-6BF403DF49AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F450C696-CD13-4974-BFDF-8C8642BB26A8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F450C696-CD13-4974-BFDF-8C8642BB26A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -198,7 +198,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,6 +217,27 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -267,19 +288,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="-0.249977111117893"/>
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -373,10 +393,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -428,28 +451,42 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="1" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -766,21 +803,21 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.109375" customWidth="1"/>
-    <col min="2" max="2" width="12.21875" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.5546875" customWidth="1"/>
-    <col min="23" max="23" width="10.88671875" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.5703125" customWidth="1"/>
+    <col min="23" max="23" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -845,24 +882,24 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="19"/>
-      <c r="C2" s="20">
+      <c r="C2" s="39">
         <v>45138</v>
       </c>
-      <c r="D2" s="21">
+      <c r="D2" s="40">
         <v>45145</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="40">
         <v>45152</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="40">
         <v>45159</v>
       </c>
-      <c r="G2" s="21">
+      <c r="G2" s="41">
         <v>45166</v>
       </c>
       <c r="H2" s="21">
@@ -908,11 +945,11 @@
         <v>45264</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="31"/>
+      <c r="B3" s="38"/>
       <c r="C3" s="10"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
@@ -936,9 +973,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="29" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="2"/>
@@ -950,11 +987,11 @@
       <c r="V4" t="s">
         <v>47</v>
       </c>
-      <c r="W4" s="9"/>
-    </row>
-    <row r="5" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W4" s="34"/>
+    </row>
+    <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="30" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="5"/>
@@ -981,11 +1018,11 @@
       </c>
       <c r="W5" s="27"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A6" s="30" t="s">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="31"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="10"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
@@ -1010,24 +1047,24 @@
       </c>
       <c r="W6" s="26"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="J7" s="14"/>
+      <c r="J7" s="36"/>
       <c r="K7" s="2"/>
       <c r="M7" s="4"/>
       <c r="U7" s="4"/>
       <c r="V7" t="s">
         <v>51</v>
       </c>
-      <c r="W7" s="29"/>
-    </row>
-    <row r="8" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W7" s="28"/>
+    </row>
+    <row r="8" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="30" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="5"/>
@@ -1050,11 +1087,11 @@
       <c r="T8" s="6"/>
       <c r="U8" s="8"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A9" s="30" t="s">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="31"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="10"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
@@ -1077,23 +1114,23 @@
       <c r="V9" t="s">
         <v>49</v>
       </c>
-      <c r="W9" s="28"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W9" s="33"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="31" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="E10" s="27"/>
+      <c r="E10" s="32"/>
       <c r="J10" s="4"/>
       <c r="K10" s="2"/>
       <c r="M10" s="4"/>
       <c r="U10" s="4"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="29" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="2"/>
@@ -1102,9 +1139,9 @@
       <c r="M11" s="4"/>
       <c r="U11" s="4"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="29" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="2"/>
@@ -1113,9 +1150,9 @@
       <c r="M12" s="14"/>
       <c r="U12" s="4"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="29" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="2"/>
@@ -1125,9 +1162,9 @@
       <c r="R13" s="9"/>
       <c r="U13" s="4"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="29" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="2"/>
@@ -1137,9 +1174,9 @@
       <c r="R14" s="9"/>
       <c r="U14" s="4"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="29" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="2"/>
@@ -1149,9 +1186,9 @@
       <c r="S15" s="9"/>
       <c r="U15" s="4"/>
     </row>
-    <row r="16" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="30" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="5"/>
@@ -1174,11 +1211,11 @@
       <c r="T16" s="7"/>
       <c r="U16" s="8"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A17" s="30" t="s">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="31"/>
+      <c r="B17" s="38"/>
       <c r="C17" s="10"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
@@ -1199,9 +1236,9 @@
       <c r="T17" s="11"/>
       <c r="U17" s="12"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="29" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="2"/>
@@ -1210,9 +1247,9 @@
       <c r="M18" s="4"/>
       <c r="U18" s="4"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="29" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="2"/>
@@ -1222,9 +1259,9 @@
       <c r="O19" s="9"/>
       <c r="U19" s="4"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="29" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="2"/>
@@ -1234,9 +1271,9 @@
       <c r="T20" s="9"/>
       <c r="U20" s="4"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="29" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="2"/>
@@ -1246,9 +1283,9 @@
       <c r="T21" s="9"/>
       <c r="U21" s="4"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="29" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="2"/>
@@ -1258,9 +1295,9 @@
       <c r="T22" s="9"/>
       <c r="U22" s="4"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="29" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="2"/>
@@ -1270,9 +1307,9 @@
       <c r="T23" s="9"/>
       <c r="U23" s="4"/>
     </row>
-    <row r="24" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="29" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="2"/>
@@ -1281,11 +1318,11 @@
       <c r="M24" s="4"/>
       <c r="U24" s="14"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A25" s="30" t="s">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="31"/>
+      <c r="B25" s="38"/>
       <c r="C25" s="10"/>
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
@@ -1306,9 +1343,9 @@
       <c r="T25" s="11"/>
       <c r="U25" s="12"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="B26" s="33" t="s">
+      <c r="B26" s="29" t="s">
         <v>30</v>
       </c>
       <c r="C26" s="2"/>
@@ -1317,11 +1354,11 @@
       <c r="M26" s="4"/>
       <c r="U26" s="4"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="33" t="s">
+      <c r="B27" s="29" t="s">
         <v>32</v>
       </c>
       <c r="C27" s="2"/>
@@ -1331,9 +1368,9 @@
       <c r="R27" s="9"/>
       <c r="U27" s="4"/>
     </row>
-    <row r="28" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
-      <c r="B28" s="34" t="s">
+      <c r="B28" s="30" t="s">
         <v>34</v>
       </c>
       <c r="C28" s="5"/>
@@ -1356,11 +1393,11 @@
       <c r="T28" s="7"/>
       <c r="U28" s="8"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A29" s="30" t="s">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="31"/>
+      <c r="B29" s="38"/>
       <c r="C29" s="10"/>
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
@@ -1381,9 +1418,9 @@
       <c r="T29" s="11"/>
       <c r="U29" s="12"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
-      <c r="B30" s="33">
+      <c r="B30" s="29">
         <v>1</v>
       </c>
       <c r="C30" s="2"/>
@@ -1392,9 +1429,9 @@
       <c r="M30" s="4"/>
       <c r="U30" s="4"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
-      <c r="B31" s="33">
+      <c r="B31" s="29">
         <v>2</v>
       </c>
       <c r="C31" s="2"/>
@@ -1403,9 +1440,9 @@
       <c r="M31" s="4"/>
       <c r="U31" s="4"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
-      <c r="B32" s="33" t="s">
+      <c r="B32" s="29" t="s">
         <v>44</v>
       </c>
       <c r="C32" s="2"/>
@@ -1414,9 +1451,9 @@
       <c r="M32" s="4"/>
       <c r="U32" s="4"/>
     </row>
-    <row r="33" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
-      <c r="B33" s="34" t="s">
+      <c r="B33" s="30" t="s">
         <v>45</v>
       </c>
       <c r="C33" s="5"/>
@@ -1439,11 +1476,11 @@
       <c r="T33" s="6"/>
       <c r="U33" s="8"/>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A34" s="30" t="s">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="31"/>
+      <c r="B34" s="38"/>
       <c r="C34" s="10"/>
       <c r="D34" s="11"/>
       <c r="E34" s="11"/>
@@ -1464,9 +1501,9 @@
       <c r="T34" s="11"/>
       <c r="U34" s="12"/>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
-      <c r="B35" s="35" t="s">
+      <c r="B35" s="31" t="s">
         <v>30</v>
       </c>
       <c r="C35" s="2"/>
@@ -1476,9 +1513,9 @@
       <c r="M35" s="4"/>
       <c r="U35" s="4"/>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
-      <c r="B36" s="33" t="s">
+      <c r="B36" s="29" t="s">
         <v>32</v>
       </c>
       <c r="C36" s="2"/>
@@ -1488,9 +1525,9 @@
       <c r="M36" s="4"/>
       <c r="U36" s="4"/>
     </row>
-    <row r="37" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
-      <c r="B37" s="34" t="s">
+      <c r="B37" s="30" t="s">
         <v>34</v>
       </c>
       <c r="C37" s="5"/>
@@ -1513,11 +1550,11 @@
       <c r="T37" s="6"/>
       <c r="U37" s="8"/>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A38" s="30" t="s">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="31"/>
+      <c r="B38" s="38"/>
       <c r="C38" s="10"/>
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
@@ -1538,9 +1575,9 @@
       <c r="T38" s="11"/>
       <c r="U38" s="12"/>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
-      <c r="B39" s="36" t="s">
+      <c r="B39" s="31" t="s">
         <v>30</v>
       </c>
       <c r="C39" s="2"/>
@@ -1550,9 +1587,9 @@
       <c r="M39" s="4"/>
       <c r="U39" s="4"/>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
-      <c r="B40" s="33" t="s">
+      <c r="B40" s="29" t="s">
         <v>32</v>
       </c>
       <c r="C40" s="2"/>
@@ -1562,9 +1599,9 @@
       <c r="M40" s="4"/>
       <c r="U40" s="4"/>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
-      <c r="B41" s="33" t="s">
+      <c r="B41" s="29" t="s">
         <v>34</v>
       </c>
       <c r="C41" s="2"/>
@@ -1573,9 +1610,9 @@
       <c r="M41" s="4"/>
       <c r="U41" s="4"/>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
-      <c r="B42" s="33" t="s">
+      <c r="B42" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C42" s="2"/>
@@ -1585,9 +1622,9 @@
       <c r="M42" s="4"/>
       <c r="U42" s="4"/>
     </row>
-    <row r="43" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
-      <c r="B43" s="34" t="s">
+      <c r="B43" s="30" t="s">
         <v>36</v>
       </c>
       <c r="C43" s="5"/>

</xml_diff>

<commit_message>
a bunch of shit
</commit_message>
<xml_diff>
--- a/Semester02_AssessmentPlan .xlsx
+++ b/Semester02_AssessmentPlan .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre\Desktop\Tafe-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3B7113-519C-4018-B5CD-B2D768AB0494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF0A2C0-492F-45EE-8AF0-A55D074F5E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F450C696-CD13-4974-BFDF-8C8642BB26A8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
   <si>
     <t>Subject</t>
   </si>
@@ -172,24 +172,6 @@
   </si>
   <si>
     <t>4 (TBC)</t>
-  </si>
-  <si>
-    <t>Key</t>
-  </si>
-  <si>
-    <t>Due in future</t>
-  </si>
-  <si>
-    <t>Completed</t>
-  </si>
-  <si>
-    <t>OverDue</t>
-  </si>
-  <si>
-    <t>Completed-Passed</t>
-  </si>
-  <si>
-    <t>Completed-Failed</t>
   </si>
   <si>
     <t>=IF(WEEKNUM(TODAY())==WEEKNUM(C2))</t>
@@ -251,7 +233,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,18 +267,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -406,9 +376,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -439,9 +409,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -452,37 +420,41 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="2" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="4" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -496,7 +468,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
+          <bgColor theme="7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -510,7 +482,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7"/>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -824,11 +796,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D027B5-64ED-4564-9511-705E2CE1AE53}">
-  <dimension ref="A1:W43"/>
+  <dimension ref="A1:V43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J30" sqref="J30"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V25" sqref="V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -844,35 +816,35 @@
     <col min="23" max="23" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="H1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="31" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="13" t="s">
@@ -884,32 +856,32 @@
       <c r="M1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="33" t="s">
+      <c r="N1" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="33" t="s">
+      <c r="O1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="P1" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="33" t="s">
+      <c r="Q1" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="R1" s="33" t="s">
+      <c r="R1" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="33" t="s">
+      <c r="S1" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="33" t="s">
+      <c r="T1" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="33" t="s">
+      <c r="U1" s="28" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>15</v>
       </c>
@@ -926,7 +898,7 @@
       <c r="F2" s="11">
         <v>45159</v>
       </c>
-      <c r="G2" s="32">
+      <c r="G2" s="27">
         <v>45166</v>
       </c>
       <c r="H2" s="11">
@@ -972,7 +944,7 @@
         <v>45264</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="38" t="s">
         <v>43</v>
       </c>
@@ -996,29 +968,22 @@
       <c r="S3" s="7"/>
       <c r="T3" s="7"/>
       <c r="U3" s="8"/>
-      <c r="V3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="17" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="1"/>
       <c r="J4" s="2"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="29"/>
+      <c r="L4" s="25"/>
       <c r="M4" s="2"/>
       <c r="U4" s="2"/>
-      <c r="V4" t="s">
-        <v>47</v>
-      </c>
-      <c r="W4" s="24"/>
-    </row>
-    <row r="5" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="18" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="3"/>
@@ -1038,14 +1003,10 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
-      <c r="T5" s="28"/>
+      <c r="T5" s="24"/>
       <c r="U5" s="5"/>
-      <c r="V5" t="s">
-        <v>48</v>
-      </c>
-      <c r="W5" s="17"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="38" t="s">
         <v>42</v>
       </c>
@@ -1069,29 +1030,20 @@
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
       <c r="U6" s="8"/>
-      <c r="V6" t="s">
-        <v>50</v>
-      </c>
-      <c r="W6" s="16"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1"/>
       <c r="J7" s="26"/>
       <c r="K7" s="1"/>
       <c r="M7" s="2"/>
       <c r="U7" s="2"/>
-      <c r="V7" t="s">
-        <v>51</v>
-      </c>
-      <c r="W7" s="18"/>
-    </row>
-    <row r="8" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="18" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="3"/>
@@ -1102,19 +1054,18 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="5"/>
+      <c r="K8" s="1"/>
+      <c r="M8" s="2"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
-      <c r="S8" s="28"/>
+      <c r="S8" s="24"/>
       <c r="T8" s="4"/>
       <c r="U8" s="5"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="38" t="s">
         <v>41</v>
       </c>
@@ -1126,7 +1077,7 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
-      <c r="J9" s="8"/>
+      <c r="J9" s="7"/>
       <c r="K9" s="6"/>
       <c r="L9" s="7"/>
       <c r="M9" s="8"/>
@@ -1138,87 +1089,77 @@
       <c r="S9" s="7"/>
       <c r="T9" s="7"/>
       <c r="U9" s="8"/>
-      <c r="V9" t="s">
-        <v>49</v>
-      </c>
-      <c r="W9" s="23"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="19" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="E10" s="22"/>
-      <c r="J10" s="2"/>
+      <c r="E10" s="20"/>
       <c r="K10" s="1"/>
       <c r="M10" s="2"/>
       <c r="U10" s="2"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="41" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="1"/>
+      <c r="K11" s="40"/>
       <c r="M11" s="2"/>
       <c r="U11" s="2"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="17" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="J12" s="2"/>
       <c r="K12" s="1"/>
-      <c r="M12" s="26"/>
+      <c r="M12" s="22"/>
       <c r="U12" s="2"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="J13" s="2"/>
       <c r="K13" s="1"/>
       <c r="M13" s="2"/>
-      <c r="R13" s="24"/>
+      <c r="R13" s="21"/>
       <c r="U13" s="2"/>
       <c r="V13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="17" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="J14" s="2"/>
       <c r="K14" s="1"/>
       <c r="M14" s="2"/>
-      <c r="R14" s="24"/>
+      <c r="R14" s="21"/>
       <c r="U14" s="2"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="17" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="1"/>
-      <c r="J15" s="2"/>
       <c r="K15" s="1"/>
       <c r="M15" s="2"/>
-      <c r="S15" s="24"/>
+      <c r="S15" s="21"/>
       <c r="U15" s="2"/>
     </row>
-    <row r="16" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="18" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="3"/>
@@ -1228,7 +1169,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
-      <c r="J16" s="5"/>
+      <c r="J16" s="4"/>
       <c r="K16" s="3"/>
       <c r="L16" s="4"/>
       <c r="M16" s="5"/>
@@ -1238,7 +1179,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
-      <c r="T16" s="28"/>
+      <c r="T16" s="24"/>
       <c r="U16" s="5"/>
       <c r="V16" t="b">
         <f ca="1">(WEEKNUM(TODAY())=WEEKNUM(C2))</f>
@@ -1258,9 +1199,9 @@
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="8"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="8"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="37"/>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
@@ -1276,7 +1217,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="J18" s="31"/>
+      <c r="I18" s="34"/>
       <c r="K18" s="1"/>
       <c r="M18" s="2"/>
       <c r="U18" s="2"/>
@@ -1287,70 +1228,69 @@
         <v>18</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="J19" s="2"/>
+      <c r="J19" s="20"/>
       <c r="K19" s="1"/>
       <c r="M19" s="2"/>
-      <c r="O19" s="24"/>
       <c r="U19" s="2"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="17" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="1"/>
       <c r="J20" s="2"/>
       <c r="K20" s="1"/>
       <c r="M20" s="2"/>
-      <c r="T20" s="24"/>
+      <c r="T20" s="21"/>
       <c r="U20" s="2"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="1"/>
       <c r="J21" s="2"/>
       <c r="K21" s="1"/>
       <c r="M21" s="2"/>
-      <c r="T21" s="24"/>
+      <c r="T21" s="21"/>
       <c r="U21" s="2"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="17" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="1"/>
       <c r="J22" s="2"/>
       <c r="K22" s="1"/>
       <c r="M22" s="2"/>
-      <c r="T22" s="24"/>
+      <c r="T22" s="21"/>
       <c r="U22" s="2"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="17" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="1"/>
       <c r="J23" s="2"/>
       <c r="K23" s="1"/>
       <c r="M23" s="2"/>
-      <c r="T23" s="24"/>
+      <c r="T23" s="21"/>
       <c r="U23" s="2"/>
     </row>
     <row r="24" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="17" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="1"/>
       <c r="J24" s="2"/>
       <c r="K24" s="1"/>
       <c r="M24" s="2"/>
-      <c r="U24" s="26"/>
+      <c r="U24" s="22"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" s="38" t="s">
@@ -1379,7 +1319,7 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="17" t="s">
         <v>30</v>
       </c>
       <c r="C26" s="1"/>
@@ -1392,19 +1332,19 @@
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="17" t="s">
         <v>32</v>
       </c>
       <c r="C27" s="1"/>
       <c r="J27" s="2"/>
       <c r="K27" s="1"/>
       <c r="M27" s="2"/>
-      <c r="Q27" s="24"/>
+      <c r="Q27" s="21"/>
       <c r="U27" s="2"/>
     </row>
     <row r="28" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="18" t="s">
         <v>34</v>
       </c>
       <c r="C28" s="3"/>
@@ -1424,7 +1364,7 @@
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
       <c r="S28" s="4"/>
-      <c r="T28" s="28"/>
+      <c r="T28" s="24"/>
       <c r="U28" s="5"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.3">
@@ -1458,7 +1398,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="1"/>
-      <c r="J30" s="30"/>
+      <c r="J30" s="33"/>
       <c r="K30" s="1"/>
       <c r="M30" s="2"/>
       <c r="U30" s="2"/>
@@ -1469,26 +1409,26 @@
         <v>2</v>
       </c>
       <c r="C31" s="1"/>
-      <c r="H31" s="37"/>
+      <c r="H31" s="32"/>
       <c r="K31" s="1"/>
       <c r="M31" s="2"/>
       <c r="U31" s="2"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
-      <c r="B32" s="19" t="s">
+      <c r="B32" s="17" t="s">
         <v>44</v>
       </c>
       <c r="C32" s="1"/>
       <c r="J32" s="2"/>
       <c r="K32" s="1"/>
       <c r="M32" s="2"/>
-      <c r="Q32" s="24"/>
+      <c r="Q32" s="21"/>
       <c r="U32" s="2"/>
     </row>
     <row r="33" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="18" t="s">
         <v>45</v>
       </c>
       <c r="C33" s="3"/>
@@ -1509,7 +1449,7 @@
       <c r="R33" s="4"/>
       <c r="S33" s="4"/>
       <c r="T33" s="4"/>
-      <c r="U33" s="27"/>
+      <c r="U33" s="23"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" s="38" t="s">
@@ -1538,11 +1478,11 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="19" t="s">
         <v>30</v>
       </c>
       <c r="C35" s="1"/>
-      <c r="F35" s="17"/>
+      <c r="F35" s="16"/>
       <c r="J35" s="2"/>
       <c r="K35" s="1"/>
       <c r="M35" s="2"/>
@@ -1550,19 +1490,18 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="17" t="s">
         <v>32</v>
       </c>
       <c r="C36" s="1"/>
-      <c r="I36" s="24"/>
       <c r="J36" s="2"/>
-      <c r="K36" s="1"/>
+      <c r="K36" s="21"/>
       <c r="M36" s="2"/>
       <c r="U36" s="2"/>
     </row>
     <row r="37" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="18" t="s">
         <v>34</v>
       </c>
       <c r="C37" s="3"/>
@@ -1581,7 +1520,7 @@
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
       <c r="R37" s="4"/>
-      <c r="S37" s="28"/>
+      <c r="S37" s="24"/>
       <c r="T37" s="4"/>
       <c r="U37" s="5"/>
     </row>
@@ -1612,11 +1551,11 @@
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
-      <c r="B39" s="21" t="s">
+      <c r="B39" s="19" t="s">
         <v>30</v>
       </c>
       <c r="C39" s="1"/>
-      <c r="F39" s="22"/>
+      <c r="F39" s="20"/>
       <c r="J39" s="2"/>
       <c r="K39" s="1"/>
       <c r="M39" s="2"/>
@@ -1628,7 +1567,7 @@
         <v>32</v>
       </c>
       <c r="C40" s="1"/>
-      <c r="H40" s="22"/>
+      <c r="H40" s="20"/>
       <c r="J40" s="2"/>
       <c r="K40" s="1"/>
       <c r="M40" s="2"/>
@@ -1647,19 +1586,19 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="17" t="s">
         <v>35</v>
       </c>
       <c r="C42" s="1"/>
       <c r="J42" s="2"/>
       <c r="K42" s="1"/>
-      <c r="L42" s="24"/>
+      <c r="L42" s="21"/>
       <c r="M42" s="2"/>
       <c r="U42" s="2"/>
     </row>
     <row r="43" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="18" t="s">
         <v>36</v>
       </c>
       <c r="C43" s="3"/>
@@ -1672,7 +1611,7 @@
       <c r="J43" s="5"/>
       <c r="K43" s="3"/>
       <c r="L43" s="4"/>
-      <c r="M43" s="27"/>
+      <c r="M43" s="23"/>
       <c r="N43" s="4"/>
       <c r="O43" s="4"/>
       <c r="P43" s="4"/>
@@ -1694,14 +1633,14 @@
     <mergeCell ref="A9:B9"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:U2">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>WEEKNUM(TODAY())=WEEKNUM(C2)</formula>
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>WEEKNUM(TODAY())&lt;WEEKNUM(C2)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>WEEKNUM(TODAY())&gt;WEEKNUM(C2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>WEEKNUM(TODAY())&lt;WEEKNUM(C2)</formula>
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>WEEKNUM(TODAY())=WEEKNUM(C2)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Done data base side
</commit_message>
<xml_diff>
--- a/Semester02_AssessmentPlan .xlsx
+++ b/Semester02_AssessmentPlan .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Tafe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58688D2-268F-48EB-AF38-5FAE589B7465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079278FB-AF66-4297-B511-BDE302093FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F450C696-CD13-4974-BFDF-8C8642BB26A8}"/>
   </bookViews>
@@ -375,7 +375,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -448,18 +448,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
@@ -467,6 +459,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -811,8 +809,8 @@
   <dimension ref="A1:U43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z12" sqref="Z12"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,10 +955,10 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="41"/>
+      <c r="B3" s="48"/>
       <c r="C3" s="6"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -1020,10 +1018,10 @@
       <c r="U5" s="5"/>
     </row>
     <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="41"/>
+      <c r="B6" s="48"/>
       <c r="C6" s="6"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
@@ -1046,25 +1044,24 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="48"/>
-      <c r="K7" s="44"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="44"/>
       <c r="M7" s="2"/>
       <c r="N7" s="1"/>
       <c r="U7" s="2"/>
     </row>
     <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="46" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="3"/>
@@ -1075,7 +1072,6 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="44"/>
       <c r="M8" s="2"/>
       <c r="N8" s="3"/>
       <c r="O8" s="4"/>
@@ -1087,18 +1083,18 @@
       <c r="U8" s="5"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="41"/>
+      <c r="B9" s="48"/>
       <c r="C9" s="33"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="45"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
       <c r="K9" s="6"/>
       <c r="L9" s="7"/>
       <c r="M9" s="8"/>
@@ -1147,14 +1143,14 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="41" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="1"/>
       <c r="K13" s="1"/>
       <c r="M13" s="2"/>
       <c r="N13" s="1"/>
-      <c r="R13" s="42"/>
+      <c r="R13" s="40"/>
       <c r="U13" s="2"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -1207,10 +1203,10 @@
       <c r="U16" s="5"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="41"/>
+      <c r="B17" s="48"/>
       <c r="C17" s="6"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -1320,10 +1316,10 @@
       <c r="U24" s="21"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="40" t="s">
+      <c r="A25" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="41"/>
+      <c r="B25" s="48"/>
       <c r="C25" s="6"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
@@ -1397,10 +1393,10 @@
       <c r="U28" s="5"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="41"/>
+      <c r="B29" s="48"/>
       <c r="C29" s="6"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
@@ -1484,10 +1480,10 @@
       <c r="U33" s="22"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="40" t="s">
+      <c r="A34" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="41"/>
+      <c r="B34" s="48"/>
       <c r="C34" s="6"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
@@ -1523,14 +1519,14 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="19" t="s">
         <v>32</v>
       </c>
       <c r="C36" s="1"/>
       <c r="J36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="1"/>
-      <c r="Q36" s="36"/>
+      <c r="Q36" s="32"/>
       <c r="U36" s="2"/>
     </row>
     <row r="37" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1559,10 +1555,10 @@
       <c r="U37" s="5"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="40" t="s">
+      <c r="A38" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="41"/>
+      <c r="B38" s="48"/>
       <c r="C38" s="6"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>

</xml_diff>